<commit_message>
penyelesaian fitur template standar biaya
</commit_message>
<xml_diff>
--- a/template/Template Biaya Penginapan Dalam Kota_Kabupaten.xlsx
+++ b/template/Template Biaya Penginapan Dalam Kota_Kabupaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Belajar Coding _Programmer\aplikasi-perjadin\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4155E28-9911-46AE-B2C2-6C9F11C07689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B828ED-4036-4413-ADE2-D7ECEB579A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DEF48955-3BAF-4228-8703-FD2D8BD68B24}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>NO</t>
   </si>
@@ -55,6 +55,36 @@
   </si>
   <si>
     <t>Tanah Pinoh Barat</t>
+  </si>
+  <si>
+    <t>Tanah Pinoh</t>
+  </si>
+  <si>
+    <t>Sokan</t>
+  </si>
+  <si>
+    <t>Sayan</t>
+  </si>
+  <si>
+    <t>Menukung</t>
+  </si>
+  <si>
+    <t>Ella Hilir</t>
+  </si>
+  <si>
+    <t>Pinoh Selatan</t>
+  </si>
+  <si>
+    <t>Pinoh Utara</t>
+  </si>
+  <si>
+    <t>Belimbing</t>
+  </si>
+  <si>
+    <t>Belimbing Hulu</t>
+  </si>
+  <si>
+    <t>Nanga Pinoh</t>
   </si>
 </sst>
 </file>
@@ -64,7 +94,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +105,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -101,22 +144,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -432,28 +484,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B390032-B230-4A08-864F-BDA9F30DEB48}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="8" max="8" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="6" style="5" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" style="5" customWidth="1"/>
+    <col min="4" max="7" width="8.7265625" style="5"/>
+    <col min="8" max="8" width="25.453125" style="5" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -465,73 +519,276 @@
       <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="1" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6">
-        <v>350000</v>
-      </c>
-      <c r="E3" s="6">
-        <v>300000</v>
-      </c>
-      <c r="F3" s="6">
-        <v>275000</v>
-      </c>
-      <c r="G3" s="6">
-        <v>250000</v>
-      </c>
-      <c r="H3" s="2"/>
+      <c r="C3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E3" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F3" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G3" s="9">
+        <v>250000</v>
+      </c>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E4" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F4" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G4" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E5" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F5" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G5" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E6" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F6" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G6" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E7" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F7" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G7" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E8" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F8" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G8" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E9" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F9" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G9" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E10" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F10" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G10" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E11" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F11" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G11" s="9">
+        <v>250000</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E12" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F12" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G12" s="9">
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="9">
+        <v>350000</v>
+      </c>
+      <c r="E13" s="9">
+        <v>300000</v>
+      </c>
+      <c r="F13" s="9">
+        <v>275000</v>
+      </c>
+      <c r="G13" s="9">
+        <v>250000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>